<commit_message>
notebooks: actualiza cancer_type_keywords en uimeo_data_analysis; core: progreso/logs en PubMed (bibliography.py); datos: actualiza archivos raw_data
</commit_message>
<xml_diff>
--- a/raw_data/CG-TEM-difuso.xlsx
+++ b/raw_data/CG-TEM-difuso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiocastelarfernandez/Desktop/SERVICIO SOCIAL/analisis_bioformatico/uimeo_data_analysis/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiocastelarfernandez/Desktop/CancerGeneSignatures/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C08869-7055-2440-8D4E-3AE2E06342A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B051CB-50B9-184D-9920-2EA954488BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="204">
   <si>
     <t xml:space="preserve">Código de la muestra </t>
   </si>
@@ -57,22 +57,10 @@
     <t>3CG-173</t>
   </si>
   <si>
-    <t>Muestra (Clave Interna)</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
     <t>C2</t>
-  </si>
-  <si>
-    <t>DGC1</t>
-  </si>
-  <si>
-    <t>DGC2</t>
-  </si>
-  <si>
-    <t>DGC3</t>
   </si>
   <si>
     <t>Pos</t>
@@ -764,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -793,28 +781,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -823,33 +789,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1065,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G1000"/>
+  <dimension ref="A2:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,599 +1062,601 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
+      <c r="C4" s="4">
+        <v>30.914709091186523</v>
+      </c>
+      <c r="D4" s="6">
+        <v>31.904964447021484</v>
+      </c>
+      <c r="E4" s="6">
+        <v>31.944887161254883</v>
+      </c>
+      <c r="F4" s="6">
+        <v>30.924041748046875</v>
+      </c>
+      <c r="G4" s="6">
+        <v>31.893190383911133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4">
-        <v>30.914709091186523</v>
+        <v>29.892593383789062</v>
       </c>
       <c r="D5" s="6">
-        <v>31.904964447021484</v>
+        <v>31.886123657226562</v>
       </c>
       <c r="E5" s="6">
-        <v>31.944887161254883</v>
+        <v>30.888216018676758</v>
       </c>
       <c r="F5" s="6">
-        <v>30.924041748046875</v>
+        <v>30.899114608764648</v>
       </c>
       <c r="G5" s="6">
-        <v>31.893190383911133</v>
+        <v>32.889793395996094</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4">
-        <v>29.892593383789062</v>
+        <v>29.894725799560547</v>
       </c>
       <c r="D6" s="6">
-        <v>31.886123657226562</v>
+        <v>31.893165588378906</v>
       </c>
       <c r="E6" s="6">
-        <v>30.888216018676758</v>
+        <v>30.904109954833984</v>
       </c>
       <c r="F6" s="6">
-        <v>30.899114608764648</v>
+        <v>31.908054351806641</v>
       </c>
       <c r="G6" s="6">
-        <v>32.889793395996094</v>
+        <v>34.889080047607422</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4">
+        <v>32.885646820068359</v>
+      </c>
+      <c r="D7" s="6">
+        <v>35.893211364746094</v>
+      </c>
+      <c r="E7" s="6">
+        <v>32.896457672119141</v>
+      </c>
+      <c r="F7" s="6">
+        <v>33.894626617431641</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4">
-        <v>29.894725799560547</v>
-      </c>
-      <c r="D7" s="6">
-        <v>31.893165588378906</v>
-      </c>
-      <c r="E7" s="6">
-        <v>30.904109954833984</v>
-      </c>
-      <c r="F7" s="6">
-        <v>31.908054351806641</v>
-      </c>
-      <c r="G7" s="6">
-        <v>34.889080047607422</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="4">
-        <v>32.885646820068359</v>
+        <v>31.923347473144531</v>
       </c>
       <c r="D8" s="6">
-        <v>35.893211364746094</v>
+        <v>32.907798767089844</v>
       </c>
       <c r="E8" s="6">
-        <v>32.896457672119141</v>
+        <v>30.918056488037109</v>
       </c>
       <c r="F8" s="6">
-        <v>33.894626617431641</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>23</v>
+        <v>31.931125640869141</v>
+      </c>
+      <c r="G8" s="6">
+        <v>32.939846038818359</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4">
-        <v>31.923347473144531</v>
+        <v>30.947450637817383</v>
       </c>
       <c r="D9" s="6">
-        <v>32.907798767089844</v>
+        <v>31.935949325561523</v>
       </c>
       <c r="E9" s="6">
-        <v>30.918056488037109</v>
+        <v>29.903995513916016</v>
       </c>
       <c r="F9" s="6">
-        <v>31.931125640869141</v>
+        <v>29.906711578369141</v>
       </c>
       <c r="G9" s="6">
-        <v>32.939846038818359</v>
+        <v>34.903968811035156</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4">
-        <v>30.947450637817383</v>
+        <v>30.898262023925781</v>
       </c>
       <c r="D10" s="6">
-        <v>31.935949325561523</v>
+        <v>33.893955230712891</v>
       </c>
       <c r="E10" s="6">
-        <v>29.903995513916016</v>
+        <v>30.899650573730469</v>
       </c>
       <c r="F10" s="6">
-        <v>29.906711578369141</v>
+        <v>30.897451400756836</v>
       </c>
       <c r="G10" s="6">
-        <v>34.903968811035156</v>
+        <v>35.904026031494141</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4">
-        <v>30.898262023925781</v>
+        <v>31.886405944824219</v>
       </c>
       <c r="D11" s="6">
-        <v>33.893955230712891</v>
+        <v>32.884441375732422</v>
       </c>
       <c r="E11" s="6">
-        <v>30.899650573730469</v>
+        <v>32.897541046142578</v>
       </c>
       <c r="F11" s="6">
-        <v>30.897451400756836</v>
+        <v>31.904237747192383</v>
       </c>
       <c r="G11" s="6">
-        <v>35.904026031494141</v>
+        <v>32.934093475341797</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4">
-        <v>31.886405944824219</v>
+        <v>30.895318984985352</v>
       </c>
       <c r="D12" s="6">
-        <v>32.884441375732422</v>
+        <v>33.894973754882812</v>
       </c>
       <c r="E12" s="6">
-        <v>32.897541046142578</v>
+        <v>28.898983001708984</v>
       </c>
       <c r="F12" s="6">
-        <v>31.904237747192383</v>
+        <v>30.89546012878418</v>
       </c>
       <c r="G12" s="6">
-        <v>32.934093475341797</v>
+        <v>32.928535461425781</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4">
-        <v>30.895318984985352</v>
+        <v>31.918970108032227</v>
       </c>
       <c r="D13" s="6">
-        <v>33.894973754882812</v>
+        <v>31.896621704101562</v>
       </c>
       <c r="E13" s="6">
-        <v>28.898983001708984</v>
+        <v>33.914936065673828</v>
       </c>
       <c r="F13" s="6">
-        <v>30.89546012878418</v>
+        <v>30.886768341064453</v>
       </c>
       <c r="G13" s="6">
-        <v>32.928535461425781</v>
+        <v>32.888950347900391</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4">
-        <v>31.918970108032227</v>
+        <v>30.8929443359375</v>
       </c>
       <c r="D14" s="6">
-        <v>31.896621704101562</v>
+        <v>32.887176513671875</v>
       </c>
       <c r="E14" s="6">
-        <v>33.914936065673828</v>
+        <v>30.889776229858398</v>
       </c>
       <c r="F14" s="6">
-        <v>30.886768341064453</v>
+        <v>31.890583038330078</v>
       </c>
       <c r="G14" s="6">
-        <v>32.888950347900391</v>
+        <v>33.8770751953125</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4">
-        <v>30.8929443359375</v>
+        <v>29.893756866455078</v>
       </c>
       <c r="D15" s="6">
-        <v>32.887176513671875</v>
+        <v>31.889411926269531</v>
       </c>
       <c r="E15" s="6">
-        <v>30.889776229858398</v>
+        <v>30.895397186279297</v>
       </c>
       <c r="F15" s="6">
-        <v>31.890583038330078</v>
+        <v>31.893978118896484</v>
       </c>
       <c r="G15" s="6">
-        <v>33.8770751953125</v>
+        <v>30.888149261474609</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4">
-        <v>29.893756866455078</v>
+        <v>28.907720565795898</v>
       </c>
       <c r="D16" s="6">
-        <v>31.889411926269531</v>
+        <v>32.92169189453125</v>
       </c>
       <c r="E16" s="6">
-        <v>30.895397186279297</v>
+        <v>29.922677993774414</v>
       </c>
       <c r="F16" s="6">
-        <v>31.893978118896484</v>
+        <v>29.912111282348633</v>
       </c>
       <c r="G16" s="6">
-        <v>30.888149261474609</v>
+        <v>32.920028686523438</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4">
-        <v>28.907720565795898</v>
+        <v>32.915229797363281</v>
       </c>
       <c r="D17" s="6">
-        <v>32.92169189453125</v>
+        <v>33.888580322265625</v>
       </c>
       <c r="E17" s="6">
-        <v>29.922677993774414</v>
+        <v>34.920734405517578</v>
       </c>
       <c r="F17" s="6">
-        <v>29.912111282348633</v>
+        <v>34.961376190185547</v>
       </c>
       <c r="G17" s="6">
-        <v>32.920028686523438</v>
+        <v>33.888065338134766</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4">
-        <v>32.915229797363281</v>
+        <v>31.933006286621094</v>
       </c>
       <c r="D18" s="6">
-        <v>33.888580322265625</v>
+        <v>33.923274993896484</v>
       </c>
       <c r="E18" s="6">
-        <v>34.920734405517578</v>
+        <v>31.921606063842773</v>
       </c>
       <c r="F18" s="6">
-        <v>34.961376190185547</v>
+        <v>31.931978225708008</v>
       </c>
       <c r="G18" s="6">
-        <v>33.888065338134766</v>
+        <v>34.900638580322266</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4">
+        <v>30.955327987670898</v>
+      </c>
+      <c r="D19" s="6">
+        <v>31.936540603637695</v>
+      </c>
+      <c r="E19" s="6">
+        <v>30.941642761230469</v>
+      </c>
+      <c r="F19" s="6">
+        <v>29.919883728027344</v>
+      </c>
+      <c r="G19" s="6">
+        <v>32.899021148681641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="4">
-        <v>31.933006286621094</v>
-      </c>
-      <c r="D19" s="6">
-        <v>33.923274993896484</v>
-      </c>
-      <c r="E19" s="6">
-        <v>31.921606063842773</v>
-      </c>
-      <c r="F19" s="6">
-        <v>31.931978225708008</v>
-      </c>
-      <c r="G19" s="6">
-        <v>34.900638580322266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="C20" s="4">
-        <v>30.955327987670898</v>
+        <v>29.900350570678711</v>
       </c>
       <c r="D20" s="6">
-        <v>31.936540603637695</v>
+        <v>31.898614883422852</v>
       </c>
       <c r="E20" s="6">
-        <v>30.941642761230469</v>
+        <v>29.896326065063477</v>
       </c>
       <c r="F20" s="6">
-        <v>29.919883728027344</v>
+        <v>30.896768569946289</v>
       </c>
       <c r="G20" s="6">
-        <v>32.899021148681641</v>
+        <v>31.900999069213867</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4">
-        <v>29.900350570678711</v>
+        <v>30.906478881835938</v>
       </c>
       <c r="D21" s="6">
-        <v>31.898614883422852</v>
+        <v>32.919303894042969</v>
       </c>
       <c r="E21" s="6">
-        <v>29.896326065063477</v>
+        <v>30.917032241821289</v>
       </c>
       <c r="F21" s="6">
-        <v>30.896768569946289</v>
+        <v>30.898159027099609</v>
       </c>
       <c r="G21" s="6">
-        <v>31.900999069213867</v>
+        <v>33.917892456054688</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="4">
-        <v>30.906478881835938</v>
+        <v>30.015558242797852</v>
       </c>
       <c r="D22" s="6">
-        <v>32.919303894042969</v>
+        <v>30.927665710449219</v>
       </c>
       <c r="E22" s="6">
-        <v>30.917032241821289</v>
+        <v>31.967668533325195</v>
       </c>
       <c r="F22" s="6">
-        <v>30.898159027099609</v>
+        <v>30.849819183349609</v>
       </c>
       <c r="G22" s="6">
-        <v>33.917892456054688</v>
+        <v>31.872804641723633</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4">
-        <v>30.015558242797852</v>
+        <v>29.908964157104492</v>
       </c>
       <c r="D23" s="6">
-        <v>30.927665710449219</v>
+        <v>31.888847351074219</v>
       </c>
       <c r="E23" s="6">
-        <v>31.967668533325195</v>
+        <v>31.890769958496094</v>
       </c>
       <c r="F23" s="6">
-        <v>30.849819183349609</v>
+        <v>31.899015426635742</v>
       </c>
       <c r="G23" s="6">
-        <v>31.872804641723633</v>
+        <v>36.961074829101562</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="4">
-        <v>29.908964157104492</v>
+        <v>30.877904891967773</v>
       </c>
       <c r="D24" s="6">
-        <v>31.888847351074219</v>
+        <v>34.897182464599609</v>
       </c>
       <c r="E24" s="6">
-        <v>31.890769958496094</v>
+        <v>29.887453079223633</v>
       </c>
       <c r="F24" s="6">
-        <v>31.899015426635742</v>
+        <v>29.89192008972168</v>
       </c>
       <c r="G24" s="6">
-        <v>36.961074829101562</v>
+        <v>34.88067626953125</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="4">
-        <v>30.877904891967773</v>
+        <v>31.898872375488281</v>
       </c>
       <c r="D25" s="6">
-        <v>34.897182464599609</v>
+        <v>31.901163101196289</v>
       </c>
       <c r="E25" s="6">
-        <v>29.887453079223633</v>
+        <v>29.901336669921875</v>
       </c>
       <c r="F25" s="6">
-        <v>29.89192008972168</v>
+        <v>31.908147811889648</v>
       </c>
       <c r="G25" s="6">
-        <v>34.88067626953125</v>
+        <v>33.903034210205078</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="4">
-        <v>31.898872375488281</v>
+        <v>32.899791717529297</v>
       </c>
       <c r="D26" s="6">
-        <v>31.901163101196289</v>
+        <v>33.884147644042969</v>
       </c>
       <c r="E26" s="6">
-        <v>29.901336669921875</v>
+        <v>34.891380310058594</v>
       </c>
       <c r="F26" s="6">
-        <v>31.908147811889648</v>
+        <v>35.889438629150391</v>
       </c>
       <c r="G26" s="6">
-        <v>33.903034210205078</v>
+        <v>34.887805938720703</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="4">
-        <v>32.899791717529297</v>
+        <v>31.900041580200195</v>
       </c>
       <c r="D27" s="6">
-        <v>33.884147644042969</v>
+        <v>34.907608032226562</v>
       </c>
       <c r="E27" s="6">
-        <v>34.891380310058594</v>
+        <v>31.897771835327148</v>
       </c>
       <c r="F27" s="6">
-        <v>35.889438629150391</v>
+        <v>30.898933410644531</v>
       </c>
       <c r="G27" s="6">
-        <v>34.887805938720703</v>
+        <v>33.888080596923828</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4">
-        <v>31.900041580200195</v>
+        <v>30.899215698242188</v>
       </c>
       <c r="D28" s="6">
-        <v>34.907608032226562</v>
+        <v>36.904891967773438</v>
       </c>
       <c r="E28" s="6">
-        <v>31.897771835327148</v>
+        <v>30.905134201049805</v>
       </c>
       <c r="F28" s="6">
-        <v>30.898933410644531</v>
+        <v>31.904853820800781</v>
       </c>
       <c r="G28" s="6">
-        <v>33.888080596923828</v>
+        <v>33.89794921875</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1700,1657 +1664,1635 @@
         <v>7</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4">
-        <v>30.899215698242188</v>
+        <v>31.878820419311523</v>
       </c>
       <c r="D29" s="6">
-        <v>36.904891967773438</v>
+        <v>34.905368804931641</v>
       </c>
       <c r="E29" s="6">
-        <v>30.905134201049805</v>
+        <v>30.902799606323242</v>
       </c>
       <c r="F29" s="6">
-        <v>31.904853820800781</v>
+        <v>33.942939758300781</v>
       </c>
       <c r="G29" s="6">
-        <v>33.89794921875</v>
+        <v>34.928676605224609</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4">
-        <v>31.878820419311523</v>
+        <v>28.89484977722168</v>
       </c>
       <c r="D30" s="6">
-        <v>34.905368804931641</v>
+        <v>32.888473510742188</v>
       </c>
       <c r="E30" s="6">
-        <v>30.902799606323242</v>
+        <v>29.88825798034668</v>
       </c>
       <c r="F30" s="6">
-        <v>33.942939758300781</v>
+        <v>29.893768310546875</v>
       </c>
       <c r="G30" s="6">
-        <v>34.928676605224609</v>
+        <v>32.904617309570312</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="4">
-        <v>28.89484977722168</v>
+        <v>31.881462097167969</v>
       </c>
       <c r="D31" s="6">
-        <v>32.888473510742188</v>
+        <v>33.880764007568359</v>
       </c>
       <c r="E31" s="6">
-        <v>29.88825798034668</v>
+        <v>31.885356903076172</v>
       </c>
       <c r="F31" s="6">
-        <v>29.893768310546875</v>
+        <v>31.88068962097168</v>
       </c>
       <c r="G31" s="6">
-        <v>32.904617309570312</v>
+        <v>35.881183624267578</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="4">
-        <v>31.881462097167969</v>
+        <v>29.897172927856445</v>
       </c>
       <c r="D32" s="6">
-        <v>33.880764007568359</v>
+        <v>36.9315185546875</v>
       </c>
       <c r="E32" s="6">
-        <v>31.885356903076172</v>
+        <v>30.887166976928711</v>
       </c>
       <c r="F32" s="6">
-        <v>31.88068962097168</v>
-      </c>
-      <c r="G32" s="6">
-        <v>35.881183624267578</v>
+        <v>30.889389038085938</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4">
-        <v>29.897172927856445</v>
+        <v>29.894147872924805</v>
       </c>
       <c r="D33" s="6">
-        <v>36.9315185546875</v>
+        <v>31.886775970458984</v>
       </c>
       <c r="E33" s="6">
-        <v>30.887166976928711</v>
+        <v>29.881658554077148</v>
       </c>
       <c r="F33" s="6">
-        <v>30.889389038085938</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>23</v>
+        <v>29.901626586914062</v>
+      </c>
+      <c r="G33" s="6">
+        <v>30.889045715332031</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="4">
-        <v>29.894147872924805</v>
+        <v>31.873043060302734</v>
       </c>
       <c r="D34" s="6">
-        <v>31.886775970458984</v>
+        <v>31.881858825683594</v>
       </c>
       <c r="E34" s="6">
-        <v>29.881658554077148</v>
+        <v>29.875833511352539</v>
       </c>
       <c r="F34" s="6">
-        <v>29.901626586914062</v>
+        <v>30.884695053100586</v>
       </c>
       <c r="G34" s="6">
-        <v>30.889045715332031</v>
+        <v>31.888692855834961</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" s="4">
-        <v>31.873043060302734</v>
+        <v>30.891448974609375</v>
       </c>
       <c r="D35" s="6">
-        <v>31.881858825683594</v>
+        <v>37.126407623291016</v>
       </c>
       <c r="E35" s="6">
-        <v>29.875833511352539</v>
+        <v>30.898929595947266</v>
       </c>
       <c r="F35" s="6">
-        <v>30.884695053100586</v>
-      </c>
-      <c r="G35" s="6">
-        <v>31.888692855834961</v>
+        <v>33.902755737304688</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="4">
-        <v>30.891448974609375</v>
+        <v>30.897619247436523</v>
       </c>
       <c r="D36" s="6">
-        <v>37.126407623291016</v>
+        <v>34.904136657714844</v>
       </c>
       <c r="E36" s="6">
-        <v>30.898929595947266</v>
+        <v>30.909273147583008</v>
       </c>
       <c r="F36" s="6">
-        <v>33.902755737304688</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>23</v>
+        <v>30.900754928588867</v>
+      </c>
+      <c r="G36" s="6">
+        <v>36.927059173583984</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="4">
-        <v>30.897619247436523</v>
+        <v>30.900562286376953</v>
       </c>
       <c r="D37" s="6">
-        <v>34.904136657714844</v>
+        <v>36.883716583251953</v>
       </c>
       <c r="E37" s="6">
-        <v>30.909273147583008</v>
+        <v>30.897712707519531</v>
       </c>
       <c r="F37" s="6">
-        <v>30.900754928588867</v>
+        <v>30.904699325561523</v>
       </c>
       <c r="G37" s="6">
-        <v>36.927059173583984</v>
+        <v>32.901535034179688</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4">
-        <v>30.900562286376953</v>
+        <v>29.881351470947266</v>
       </c>
       <c r="D38" s="6">
-        <v>36.883716583251953</v>
+        <v>31.886241912841797</v>
       </c>
       <c r="E38" s="6">
-        <v>30.897712707519531</v>
+        <v>30.892871856689453</v>
       </c>
       <c r="F38" s="6">
-        <v>30.904699325561523</v>
+        <v>30.880392074584961</v>
       </c>
       <c r="G38" s="6">
-        <v>32.901535034179688</v>
+        <v>33.901962280273438</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="4">
-        <v>29.881351470947266</v>
+        <v>32.893413543701172</v>
       </c>
       <c r="D39" s="6">
-        <v>31.886241912841797</v>
+        <v>33.896392822265625</v>
       </c>
       <c r="E39" s="6">
-        <v>30.892871856689453</v>
+        <v>30.886276245117188</v>
       </c>
       <c r="F39" s="6">
-        <v>30.880392074584961</v>
+        <v>30.903369903564453</v>
       </c>
       <c r="G39" s="6">
-        <v>33.901962280273438</v>
+        <v>36.980171203613281</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="4">
-        <v>32.893413543701172</v>
+        <v>30.899877548217773</v>
       </c>
       <c r="D40" s="6">
-        <v>33.896392822265625</v>
+        <v>33.934902191162109</v>
       </c>
       <c r="E40" s="6">
-        <v>30.886276245117188</v>
+        <v>30.903823852539062</v>
       </c>
       <c r="F40" s="6">
-        <v>30.903369903564453</v>
+        <v>32.9139404296875</v>
       </c>
       <c r="G40" s="6">
-        <v>36.980171203613281</v>
+        <v>32.94281005859375</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4">
-        <v>30.899877548217773</v>
+        <v>29.900217056274414</v>
       </c>
       <c r="D41" s="6">
-        <v>33.934902191162109</v>
+        <v>32.897750854492188</v>
       </c>
       <c r="E41" s="6">
-        <v>30.903823852539062</v>
+        <v>29.89166259765625</v>
       </c>
       <c r="F41" s="6">
-        <v>32.9139404296875</v>
+        <v>29.888437271118164</v>
       </c>
       <c r="G41" s="6">
-        <v>32.94281005859375</v>
+        <v>30.894031524658203</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" s="4">
-        <v>29.900217056274414</v>
+        <v>30.901157379150391</v>
       </c>
       <c r="D42" s="6">
-        <v>32.897750854492188</v>
+        <v>32.888126373291016</v>
       </c>
       <c r="E42" s="6">
-        <v>29.89166259765625</v>
+        <v>30.908309936523438</v>
       </c>
       <c r="F42" s="6">
-        <v>29.888437271118164</v>
+        <v>30.896390914916992</v>
       </c>
       <c r="G42" s="6">
-        <v>30.894031524658203</v>
+        <v>32.895618438720703</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="4">
-        <v>30.901157379150391</v>
+        <v>29.90745735168457</v>
       </c>
       <c r="D43" s="6">
-        <v>32.888126373291016</v>
+        <v>33.896732330322266</v>
       </c>
       <c r="E43" s="6">
-        <v>30.908309936523438</v>
+        <v>29.895254135131836</v>
       </c>
       <c r="F43" s="6">
-        <v>30.896390914916992</v>
+        <v>30.925182342529297</v>
       </c>
       <c r="G43" s="6">
-        <v>32.895618438720703</v>
+        <v>32.928295135498047</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="4">
-        <v>29.90745735168457</v>
+        <v>30.895229339599609</v>
       </c>
       <c r="D44" s="6">
-        <v>33.896732330322266</v>
+        <v>31.896675109863281</v>
       </c>
       <c r="E44" s="6">
-        <v>29.895254135131836</v>
+        <v>29.892915725708008</v>
       </c>
       <c r="F44" s="6">
-        <v>30.925182342529297</v>
+        <v>29.903074264526367</v>
       </c>
       <c r="G44" s="6">
-        <v>32.928295135498047</v>
+        <v>32.8919677734375</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="4">
-        <v>30.895229339599609</v>
+        <v>29.884521484375</v>
       </c>
       <c r="D45" s="6">
-        <v>31.896675109863281</v>
+        <v>31.883832931518555</v>
       </c>
       <c r="E45" s="6">
-        <v>29.892915725708008</v>
+        <v>30.88783073425293</v>
       </c>
       <c r="F45" s="6">
-        <v>29.903074264526367</v>
+        <v>30.892656326293945</v>
       </c>
       <c r="G45" s="6">
-        <v>32.8919677734375</v>
+        <v>31.878406524658203</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="4">
-        <v>29.884521484375</v>
+        <v>31.918445587158203</v>
       </c>
       <c r="D46" s="6">
-        <v>31.883832931518555</v>
+        <v>31.912065505981445</v>
       </c>
       <c r="E46" s="6">
-        <v>30.88783073425293</v>
+        <v>30.913585662841797</v>
       </c>
       <c r="F46" s="6">
-        <v>30.892656326293945</v>
+        <v>31.93153190612793</v>
       </c>
       <c r="G46" s="6">
-        <v>31.878406524658203</v>
+        <v>35.903583526611328</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" s="4">
-        <v>31.918445587158203</v>
+        <v>30.92442512512207</v>
       </c>
       <c r="D47" s="6">
-        <v>31.912065505981445</v>
+        <v>32.899658203125</v>
       </c>
       <c r="E47" s="6">
-        <v>30.913585662841797</v>
+        <v>29.903505325317383</v>
       </c>
       <c r="F47" s="6">
-        <v>31.93153190612793</v>
+        <v>31.915748596191406</v>
       </c>
       <c r="G47" s="6">
-        <v>35.903583526611328</v>
+        <v>35.901119232177734</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" s="4">
-        <v>30.92442512512207</v>
+        <v>32.91314697265625</v>
       </c>
       <c r="D48" s="6">
-        <v>32.899658203125</v>
+        <v>34.887336730957031</v>
       </c>
       <c r="E48" s="6">
-        <v>29.903505325317383</v>
+        <v>32.892467498779297</v>
       </c>
       <c r="F48" s="6">
-        <v>31.915748596191406</v>
+        <v>33.901477813720703</v>
       </c>
       <c r="G48" s="6">
-        <v>35.901119232177734</v>
+        <v>34.909297943115234</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="4">
-        <v>32.91314697265625</v>
+        <v>30.918905258178711</v>
       </c>
       <c r="D49" s="6">
-        <v>34.887336730957031</v>
+        <v>32.884014129638672</v>
       </c>
       <c r="E49" s="6">
-        <v>32.892467498779297</v>
+        <v>30.898843765258789</v>
       </c>
       <c r="F49" s="6">
-        <v>33.901477813720703</v>
+        <v>30.910465240478516</v>
       </c>
       <c r="G49" s="6">
-        <v>34.909297943115234</v>
+        <v>31.909206390380859</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" s="4">
-        <v>30.918905258178711</v>
+        <v>29.917095184326172</v>
       </c>
       <c r="D50" s="6">
-        <v>32.884014129638672</v>
+        <v>33.905323028564453</v>
       </c>
       <c r="E50" s="6">
-        <v>30.898843765258789</v>
+        <v>31.950088500976562</v>
       </c>
       <c r="F50" s="6">
-        <v>30.910465240478516</v>
+        <v>29.903408050537109</v>
       </c>
       <c r="G50" s="6">
-        <v>31.909206390380859</v>
+        <v>33.912433624267578</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="4">
-        <v>29.917095184326172</v>
+        <v>31.908161163330078</v>
       </c>
       <c r="D51" s="6">
-        <v>33.905323028564453</v>
+        <v>33.892562866210938</v>
       </c>
       <c r="E51" s="6">
-        <v>31.950088500976562</v>
+        <v>31.903463363647461</v>
       </c>
       <c r="F51" s="6">
-        <v>29.903408050537109</v>
+        <v>31.899259567260742</v>
       </c>
       <c r="G51" s="6">
-        <v>33.912433624267578</v>
+        <v>34.882923126220703</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" s="4">
-        <v>31.908161163330078</v>
+        <v>29.913234710693359</v>
       </c>
       <c r="D52" s="6">
-        <v>33.892562866210938</v>
+        <v>34.909709930419922</v>
       </c>
       <c r="E52" s="6">
-        <v>31.903463363647461</v>
+        <v>30.909652709960938</v>
       </c>
       <c r="F52" s="6">
-        <v>31.899259567260742</v>
+        <v>29.910564422607422</v>
       </c>
       <c r="G52" s="6">
-        <v>34.882923126220703</v>
+        <v>33.9119873046875</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C53" s="4">
-        <v>29.913234710693359</v>
+        <v>30.884122848510742</v>
       </c>
       <c r="D53" s="6">
-        <v>34.909709930419922</v>
+        <v>32.905452728271484</v>
       </c>
       <c r="E53" s="6">
-        <v>30.909652709960938</v>
+        <v>29.896446228027344</v>
       </c>
       <c r="F53" s="6">
-        <v>29.910564422607422</v>
+        <v>29.893566131591797</v>
       </c>
       <c r="G53" s="6">
-        <v>33.9119873046875</v>
+        <v>31.887475967407227</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C54" s="4">
-        <v>30.884122848510742</v>
+        <v>30.917659759521484</v>
       </c>
       <c r="D54" s="6">
-        <v>32.905452728271484</v>
+        <v>31.892589569091797</v>
       </c>
       <c r="E54" s="6">
-        <v>29.896446228027344</v>
+        <v>30.916208267211914</v>
       </c>
       <c r="F54" s="6">
-        <v>29.893566131591797</v>
-      </c>
-      <c r="G54" s="6">
-        <v>31.887475967407227</v>
+        <v>30.907434463500977</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C55" s="4">
-        <v>30.917659759521484</v>
+        <v>29.908811569213867</v>
       </c>
       <c r="D55" s="6">
-        <v>31.892589569091797</v>
+        <v>30.887819290161133</v>
       </c>
       <c r="E55" s="6">
-        <v>30.916208267211914</v>
+        <v>28.899948120117188</v>
       </c>
       <c r="F55" s="6">
-        <v>30.907434463500977</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>23</v>
+        <v>29.892614364624023</v>
+      </c>
+      <c r="G55" s="6">
+        <v>33.924018859863281</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C56" s="4">
-        <v>29.908811569213867</v>
+        <v>29.892829895019531</v>
       </c>
       <c r="D56" s="6">
-        <v>30.887819290161133</v>
+        <v>31.896415710449219</v>
       </c>
       <c r="E56" s="6">
-        <v>28.899948120117188</v>
+        <v>29.8841552734375</v>
       </c>
       <c r="F56" s="6">
-        <v>29.892614364624023</v>
+        <v>31.879222869873047</v>
       </c>
       <c r="G56" s="6">
-        <v>33.924018859863281</v>
+        <v>31.892574310302734</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C57" s="4">
-        <v>29.892829895019531</v>
+        <v>29.896526336669922</v>
       </c>
       <c r="D57" s="6">
-        <v>31.896415710449219</v>
+        <v>33.901424407958984</v>
       </c>
       <c r="E57" s="6">
-        <v>29.8841552734375</v>
+        <v>28.896566390991211</v>
       </c>
       <c r="F57" s="6">
-        <v>31.879222869873047</v>
+        <v>30.894662857055664</v>
       </c>
       <c r="G57" s="6">
-        <v>31.892574310302734</v>
+        <v>32.898307800292969</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C58" s="4">
-        <v>29.896526336669922</v>
+        <v>30.896093368530273</v>
       </c>
       <c r="D58" s="6">
-        <v>33.901424407958984</v>
+        <v>32.882106781005859</v>
       </c>
       <c r="E58" s="6">
-        <v>28.896566390991211</v>
+        <v>30.890649795532227</v>
       </c>
       <c r="F58" s="6">
-        <v>30.894662857055664</v>
-      </c>
-      <c r="G58" s="6">
-        <v>32.898307800292969</v>
+        <v>30.890266418457031</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C59" s="4">
-        <v>30.896093368530273</v>
+        <v>29.888259887695312</v>
       </c>
       <c r="D59" s="6">
-        <v>32.882106781005859</v>
+        <v>31.891929626464844</v>
       </c>
       <c r="E59" s="6">
-        <v>30.890649795532227</v>
+        <v>29.890764236450195</v>
       </c>
       <c r="F59" s="6">
-        <v>30.890266418457031</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>23</v>
+        <v>29.890769958496094</v>
+      </c>
+      <c r="G59" s="6">
+        <v>36.922348022460938</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C60" s="4">
-        <v>29.888259887695312</v>
+        <v>29.89727783203125</v>
       </c>
       <c r="D60" s="6">
-        <v>31.891929626464844</v>
+        <v>37.016422271728516</v>
       </c>
       <c r="E60" s="6">
-        <v>29.890764236450195</v>
+        <v>29.900444030761719</v>
       </c>
       <c r="F60" s="6">
-        <v>29.890769958496094</v>
+        <v>30.896125793457031</v>
       </c>
       <c r="G60" s="6">
-        <v>36.922348022460938</v>
+        <v>33.907474517822266</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61" s="4">
-        <v>29.89727783203125</v>
+        <v>33.921558380126953</v>
       </c>
       <c r="D61" s="6">
-        <v>37.016422271728516</v>
+        <v>33.895420074462891</v>
       </c>
       <c r="E61" s="6">
-        <v>29.900444030761719</v>
+        <v>33.935703277587891</v>
       </c>
       <c r="F61" s="6">
-        <v>30.896125793457031</v>
+        <v>33.931087493896484</v>
       </c>
       <c r="G61" s="6">
-        <v>33.907474517822266</v>
+        <v>34.883781433105469</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C62" s="4">
-        <v>33.921558380126953</v>
+        <v>29.895294189453125</v>
       </c>
       <c r="D62" s="6">
-        <v>33.895420074462891</v>
+        <v>31.892704010009766</v>
       </c>
       <c r="E62" s="6">
-        <v>33.935703277587891</v>
+        <v>31.889612197875977</v>
       </c>
       <c r="F62" s="6">
-        <v>33.931087493896484</v>
+        <v>29.892343521118164</v>
       </c>
       <c r="G62" s="6">
-        <v>34.883781433105469</v>
+        <v>37.132083892822266</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C63" s="4">
-        <v>29.895294189453125</v>
+        <v>30.923200607299805</v>
       </c>
       <c r="D63" s="6">
-        <v>31.892704010009766</v>
+        <v>31.905191421508789</v>
       </c>
       <c r="E63" s="6">
-        <v>31.889612197875977</v>
+        <v>30.918914794921875</v>
       </c>
       <c r="F63" s="6">
-        <v>29.892343521118164</v>
+        <v>30.900735855102539</v>
       </c>
       <c r="G63" s="6">
-        <v>37.132083892822266</v>
+        <v>32.891578674316406</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C64" s="4">
-        <v>30.923200607299805</v>
+        <v>31.893083572387695</v>
       </c>
       <c r="D64" s="6">
-        <v>31.905191421508789</v>
+        <v>36.898963928222656</v>
       </c>
       <c r="E64" s="6">
-        <v>30.918914794921875</v>
+        <v>31.891819000244141</v>
       </c>
       <c r="F64" s="6">
-        <v>30.900735855102539</v>
+        <v>31.89398193359375</v>
       </c>
       <c r="G64" s="6">
-        <v>32.891578674316406</v>
+        <v>37.051132202148438</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C65" s="4">
-        <v>31.893083572387695</v>
+        <v>30.898645401000977</v>
       </c>
       <c r="D65" s="6">
-        <v>36.898963928222656</v>
+        <v>34.907726287841797</v>
       </c>
       <c r="E65" s="6">
-        <v>31.891819000244141</v>
+        <v>29.901870727539062</v>
       </c>
       <c r="F65" s="6">
-        <v>31.89398193359375</v>
+        <v>30.895246505737305</v>
       </c>
       <c r="G65" s="6">
-        <v>37.051132202148438</v>
+        <v>33.897579193115234</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C66" s="4">
-        <v>30.898645401000977</v>
+        <v>29.902156829833984</v>
       </c>
       <c r="D66" s="6">
-        <v>34.907726287841797</v>
+        <v>34.888587951660156</v>
       </c>
       <c r="E66" s="6">
-        <v>29.901870727539062</v>
+        <v>29.901678085327148</v>
       </c>
       <c r="F66" s="6">
-        <v>30.895246505737305</v>
+        <v>30.912179946899414</v>
       </c>
       <c r="G66" s="6">
-        <v>33.897579193115234</v>
+        <v>32.907543182373047</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C67" s="4">
-        <v>29.902156829833984</v>
+        <v>30.891826629638672</v>
       </c>
       <c r="D67" s="6">
-        <v>34.888587951660156</v>
+        <v>31.89521598815918</v>
       </c>
       <c r="E67" s="6">
-        <v>29.901678085327148</v>
+        <v>31.896270751953125</v>
       </c>
       <c r="F67" s="6">
-        <v>30.912179946899414</v>
+        <v>30.8941650390625</v>
       </c>
       <c r="G67" s="6">
-        <v>32.907543182373047</v>
+        <v>33.903182983398438</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C68" s="4">
-        <v>30.891826629638672</v>
+        <v>29.897747039794922</v>
       </c>
       <c r="D68" s="6">
-        <v>31.89521598815918</v>
+        <v>34.897499084472656</v>
       </c>
       <c r="E68" s="6">
-        <v>31.896270751953125</v>
+        <v>30.898599624633789</v>
       </c>
       <c r="F68" s="6">
-        <v>30.8941650390625</v>
+        <v>31.901504516601562</v>
       </c>
       <c r="G68" s="6">
-        <v>33.903182983398438</v>
+        <v>37.072517395019531</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C69" s="4">
-        <v>29.897747039794922</v>
+        <v>30.894525527954102</v>
       </c>
       <c r="D69" s="6">
-        <v>34.897499084472656</v>
+        <v>32.898727416992188</v>
       </c>
       <c r="E69" s="6">
-        <v>30.898599624633789</v>
+        <v>30.894599914550781</v>
       </c>
       <c r="F69" s="6">
-        <v>31.901504516601562</v>
+        <v>30.885881423950195</v>
       </c>
       <c r="G69" s="6">
-        <v>37.072517395019531</v>
+        <v>32.900722503662109</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C70" s="4">
-        <v>30.894525527954102</v>
+        <v>29.8870849609375</v>
       </c>
       <c r="D70" s="6">
-        <v>32.898727416992188</v>
+        <v>32.897296905517578</v>
       </c>
       <c r="E70" s="6">
-        <v>30.894599914550781</v>
+        <v>29.886270523071289</v>
       </c>
       <c r="F70" s="6">
-        <v>30.885881423950195</v>
+        <v>29.888147354125977</v>
       </c>
       <c r="G70" s="6">
-        <v>32.900722503662109</v>
+        <v>32.914726257324219</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C71" s="4">
-        <v>29.8870849609375</v>
+        <v>29.895362854003906</v>
       </c>
       <c r="D71" s="6">
-        <v>32.897296905517578</v>
+        <v>31.888404846191406</v>
       </c>
       <c r="E71" s="6">
-        <v>29.886270523071289</v>
+        <v>30.885124206542969</v>
       </c>
       <c r="F71" s="6">
-        <v>29.888147354125977</v>
+        <v>30.884881973266602</v>
       </c>
       <c r="G71" s="6">
-        <v>32.914726257324219</v>
+        <v>33.884727478027344</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C72" s="4">
-        <v>29.895362854003906</v>
+        <v>30.885660171508789</v>
       </c>
       <c r="D72" s="6">
-        <v>31.888404846191406</v>
+        <v>32.896446228027344</v>
       </c>
       <c r="E72" s="6">
-        <v>30.885124206542969</v>
+        <v>29.897609710693359</v>
       </c>
       <c r="F72" s="6">
-        <v>30.884881973266602</v>
+        <v>29.891565322875977</v>
       </c>
       <c r="G72" s="6">
-        <v>33.884727478027344</v>
+        <v>32.884204864501953</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C73" s="4">
-        <v>30.885660171508789</v>
+        <v>29.884965896606445</v>
       </c>
       <c r="D73" s="6">
-        <v>32.896446228027344</v>
+        <v>32.907756805419922</v>
       </c>
       <c r="E73" s="6">
-        <v>29.897609710693359</v>
+        <v>29.894618988037109</v>
       </c>
       <c r="F73" s="6">
-        <v>29.891565322875977</v>
+        <v>30.897073745727539</v>
       </c>
       <c r="G73" s="6">
-        <v>32.884204864501953</v>
+        <v>30.883157730102539</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C74" s="4">
-        <v>29.884965896606445</v>
+        <v>30.880331039428711</v>
       </c>
       <c r="D74" s="6">
-        <v>32.907756805419922</v>
+        <v>31.880773544311523</v>
       </c>
       <c r="E74" s="6">
-        <v>29.894618988037109</v>
+        <v>30.884374618530273</v>
       </c>
       <c r="F74" s="6">
-        <v>30.897073745727539</v>
+        <v>30.889837265014648</v>
       </c>
       <c r="G74" s="6">
-        <v>30.883157730102539</v>
+        <v>33.882003784179688</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C75" s="4">
-        <v>30.880331039428711</v>
+        <v>31.892080307006836</v>
       </c>
       <c r="D75" s="6">
-        <v>31.880773544311523</v>
+        <v>32.884494781494141</v>
       </c>
       <c r="E75" s="6">
-        <v>30.884374618530273</v>
+        <v>32.90472412109375</v>
       </c>
       <c r="F75" s="6">
-        <v>30.889837265014648</v>
+        <v>32.895816802978516</v>
       </c>
       <c r="G75" s="6">
-        <v>33.882003784179688</v>
+        <v>31.891382217407227</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C76" s="4">
-        <v>31.892080307006836</v>
+        <v>28.896696090698242</v>
       </c>
       <c r="D76" s="6">
-        <v>32.884494781494141</v>
+        <v>32.928638458251953</v>
       </c>
       <c r="E76" s="6">
-        <v>32.90472412109375</v>
+        <v>30.899362564086914</v>
       </c>
       <c r="F76" s="6">
-        <v>32.895816802978516</v>
+        <v>30.892740249633789</v>
       </c>
       <c r="G76" s="6">
-        <v>31.891382217407227</v>
+        <v>32.915622711181641</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C77" s="4">
-        <v>28.896696090698242</v>
+        <v>30.887510299682617</v>
       </c>
       <c r="D77" s="6">
-        <v>32.928638458251953</v>
+        <v>33.896533966064453</v>
       </c>
       <c r="E77" s="6">
-        <v>30.899362564086914</v>
+        <v>30.889188766479492</v>
       </c>
       <c r="F77" s="6">
-        <v>30.892740249633789</v>
+        <v>30.893342971801758</v>
       </c>
       <c r="G77" s="6">
-        <v>32.915622711181641</v>
+        <v>33.931838989257812</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C78" s="4">
-        <v>30.887510299682617</v>
+        <v>30.925548553466797</v>
       </c>
       <c r="D78" s="6">
-        <v>33.896533966064453</v>
+        <v>30.906772613525391</v>
       </c>
       <c r="E78" s="6">
-        <v>30.889188766479492</v>
+        <v>30.919162750244141</v>
       </c>
       <c r="F78" s="6">
-        <v>30.893342971801758</v>
+        <v>29.903596878051758</v>
       </c>
       <c r="G78" s="6">
-        <v>33.931838989257812</v>
+        <v>31.908365249633789</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C79" s="4">
-        <v>30.925548553466797</v>
+        <v>161</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D79" s="6">
-        <v>30.906772613525391</v>
+        <v>33.898845672607422</v>
       </c>
       <c r="E79" s="6">
-        <v>30.919162750244141</v>
+        <v>33.895893096923828</v>
       </c>
       <c r="F79" s="6">
-        <v>29.903596878051758</v>
-      </c>
-      <c r="G79" s="6">
-        <v>31.908365249633789</v>
+        <v>33.893379211425781</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80" s="6">
-        <v>33.898845672607422</v>
+        <v>163</v>
+      </c>
+      <c r="C80" s="4">
+        <v>29.899961471557617</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E80" s="6">
-        <v>33.895893096923828</v>
+        <v>29.899171829223633</v>
       </c>
       <c r="F80" s="6">
-        <v>33.893379211425781</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>23</v>
+        <v>30.885271072387695</v>
+      </c>
+      <c r="G80" s="6">
+        <v>37.02001953125</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C81" s="4">
-        <v>29.899961471557617</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>23</v>
+        <v>29.893932342529297</v>
+      </c>
+      <c r="D81" s="6">
+        <v>30.890195846557617</v>
       </c>
       <c r="E81" s="6">
-        <v>29.899171829223633</v>
+        <v>29.890100479125977</v>
       </c>
       <c r="F81" s="6">
-        <v>30.885271072387695</v>
+        <v>28.889928817749023</v>
       </c>
       <c r="G81" s="6">
-        <v>37.02001953125</v>
+        <v>32.895809173583984</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C82" s="4">
-        <v>29.893932342529297</v>
+        <v>29.902708053588867</v>
       </c>
       <c r="D82" s="6">
-        <v>30.890195846557617</v>
+        <v>31.896780014038086</v>
       </c>
       <c r="E82" s="6">
-        <v>29.890100479125977</v>
+        <v>29.916828155517578</v>
       </c>
       <c r="F82" s="6">
-        <v>28.889928817749023</v>
+        <v>30.896038055419922</v>
       </c>
       <c r="G82" s="6">
-        <v>32.895809173583984</v>
+        <v>32.893943786621094</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C83" s="4">
-        <v>29.902708053588867</v>
+        <v>33.893535614013672</v>
       </c>
       <c r="D83" s="6">
-        <v>31.896780014038086</v>
+        <v>33.886444091796875</v>
       </c>
       <c r="E83" s="6">
-        <v>29.916828155517578</v>
+        <v>34.922309875488281</v>
       </c>
       <c r="F83" s="6">
-        <v>30.896038055419922</v>
+        <v>34.912254333496094</v>
       </c>
       <c r="G83" s="6">
-        <v>32.893943786621094</v>
+        <v>33.899696350097656</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C84" s="4">
-        <v>33.893535614013672</v>
+        <v>30.882589340209961</v>
       </c>
       <c r="D84" s="6">
-        <v>33.886444091796875</v>
+        <v>33.898078918457031</v>
       </c>
       <c r="E84" s="6">
-        <v>34.922309875488281</v>
+        <v>30.894729614257812</v>
       </c>
       <c r="F84" s="6">
-        <v>34.912254333496094</v>
+        <v>32.901329040527344</v>
       </c>
       <c r="G84" s="6">
-        <v>33.899696350097656</v>
+        <v>34.893611907958984</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C85" s="4">
-        <v>30.882589340209961</v>
+        <v>30.881217956542969</v>
       </c>
       <c r="D85" s="6">
-        <v>33.898078918457031</v>
+        <v>31.943426132202148</v>
       </c>
       <c r="E85" s="6">
-        <v>30.894729614257812</v>
+        <v>30.893575668334961</v>
       </c>
       <c r="F85" s="6">
-        <v>32.901329040527344</v>
+        <v>29.892601013183594</v>
       </c>
       <c r="G85" s="6">
-        <v>34.893611907958984</v>
+        <v>33.905082702636719</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C86" s="4">
-        <v>30.881217956542969</v>
+        <v>30.893064498901367</v>
       </c>
       <c r="D86" s="6">
-        <v>31.943426132202148</v>
+        <v>34.887775421142578</v>
       </c>
       <c r="E86" s="6">
-        <v>30.893575668334961</v>
+        <v>29.893325805664062</v>
       </c>
       <c r="F86" s="6">
-        <v>29.892601013183594</v>
+        <v>31.897645950317383</v>
       </c>
       <c r="G86" s="6">
-        <v>33.905082702636719</v>
+        <v>34.888065338134766</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C87" s="4">
-        <v>30.893064498901367</v>
+        <v>28.890214920043945</v>
       </c>
       <c r="D87" s="6">
-        <v>34.887775421142578</v>
+        <v>31.910976409912109</v>
       </c>
       <c r="E87" s="6">
-        <v>29.893325805664062</v>
+        <v>28.897640228271484</v>
       </c>
       <c r="F87" s="6">
-        <v>31.897645950317383</v>
+        <v>29.883369445800781</v>
       </c>
       <c r="G87" s="6">
-        <v>34.888065338134766</v>
+        <v>30.883384704589844</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C88" s="4">
-        <v>28.890214920043945</v>
-      </c>
-      <c r="D88" s="6">
-        <v>31.910976409912109</v>
-      </c>
-      <c r="E88" s="6">
-        <v>28.897640228271484</v>
-      </c>
-      <c r="F88" s="6">
-        <v>29.883369445800781</v>
-      </c>
-      <c r="G88" s="6">
-        <v>30.883384704589844</v>
+        <v>179</v>
+      </c>
+      <c r="C88" s="7">
+        <v>27.890878677368164</v>
+      </c>
+      <c r="D88" s="8">
+        <v>30.989465713500977</v>
+      </c>
+      <c r="E88" s="8">
+        <v>26.895931243896484</v>
+      </c>
+      <c r="F88" s="8">
+        <v>27.894260406494141</v>
+      </c>
+      <c r="G88" s="8">
+        <v>31.91077995300293</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C89" s="7">
-        <v>27.890878677368164</v>
+        <v>27.904565811157227</v>
       </c>
       <c r="D89" s="8">
-        <v>30.989465713500977</v>
+        <v>31.926881790161133</v>
       </c>
       <c r="E89" s="8">
-        <v>26.895931243896484</v>
+        <v>27.922277450561523</v>
       </c>
       <c r="F89" s="8">
-        <v>27.894260406494141</v>
+        <v>29.91334342956543</v>
       </c>
       <c r="G89" s="8">
-        <v>31.91077995300293</v>
+        <v>33.9046630859375</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C90" s="7">
-        <v>27.904565811157227</v>
+        <v>26.905902862548828</v>
       </c>
       <c r="D90" s="8">
-        <v>31.926881790161133</v>
+        <v>29.889682769775391</v>
       </c>
       <c r="E90" s="8">
-        <v>27.922277450561523</v>
+        <v>26.896099090576172</v>
       </c>
       <c r="F90" s="8">
-        <v>29.91334342956543</v>
+        <v>26.893522262573242</v>
       </c>
       <c r="G90" s="8">
-        <v>33.9046630859375</v>
+        <v>29.901239395141602</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C91" s="7">
-        <v>26.905902862548828</v>
+        <v>31.900989532470703</v>
       </c>
       <c r="D91" s="8">
-        <v>29.889682769775391</v>
+        <v>35.902149200439453</v>
       </c>
       <c r="E91" s="8">
-        <v>26.896099090576172</v>
+        <v>34.899032592773438</v>
       </c>
       <c r="F91" s="8">
-        <v>26.893522262573242</v>
+        <v>33.894054412841797</v>
       </c>
       <c r="G91" s="8">
-        <v>29.901239395141602</v>
+        <v>33.906745910644531</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C92" s="7">
-        <v>31.900989532470703</v>
+        <v>28.902608871459961</v>
       </c>
       <c r="D92" s="8">
-        <v>35.902149200439453</v>
+        <v>30.902223587036133</v>
       </c>
       <c r="E92" s="8">
-        <v>34.899032592773438</v>
+        <v>27.909669876098633</v>
       </c>
       <c r="F92" s="8">
-        <v>33.894054412841797</v>
+        <v>28.907110214233398</v>
       </c>
       <c r="G92" s="8">
-        <v>33.906745910644531</v>
+        <v>31.906488418579102</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C93" s="7">
-        <v>28.902608871459961</v>
+        <v>29.915422439575195</v>
       </c>
       <c r="D93" s="8">
-        <v>30.902223587036133</v>
+        <v>32.902301788330078</v>
       </c>
       <c r="E93" s="8">
-        <v>27.909669876098633</v>
+        <v>29.916015625</v>
       </c>
       <c r="F93" s="8">
-        <v>28.907110214233398</v>
+        <v>29.902980804443359</v>
       </c>
       <c r="G93" s="8">
-        <v>31.906488418579102</v>
+        <v>31.905424118041992</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C94" s="7">
-        <v>29.915422439575195</v>
-      </c>
-      <c r="D94" s="8">
-        <v>32.902301788330078</v>
-      </c>
-      <c r="E94" s="8">
-        <v>29.916015625</v>
-      </c>
-      <c r="F94" s="8">
-        <v>29.902980804443359</v>
-      </c>
-      <c r="G94" s="8">
-        <v>31.905424118041992</v>
+        <v>191</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D94" s="10">
+        <v>34.897686004638672</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" s="10">
+        <v>36.893154144287109</v>
+      </c>
+      <c r="G94" s="10">
+        <v>37.091476440429688</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D95" s="10">
-        <v>34.897686004638672</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>23</v>
+        <v>34.893302917480469</v>
+      </c>
+      <c r="E95" s="10">
+        <v>37.120552062988281</v>
       </c>
       <c r="F95" s="10">
-        <v>36.893154144287109</v>
+        <v>36.899684906005859</v>
       </c>
       <c r="G95" s="10">
-        <v>37.091476440429688</v>
+        <v>37.082817077636719</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D96" s="10">
-        <v>34.893302917480469</v>
-      </c>
-      <c r="E96" s="10">
-        <v>37.120552062988281</v>
+        <v>34.897392272949219</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="F96" s="10">
-        <v>36.899684906005859</v>
-      </c>
-      <c r="G96" s="10">
-        <v>37.082817077636719</v>
+        <v>35.911441802978516</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" s="10">
-        <v>34.897392272949219</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F97" s="10">
-        <v>35.911441802978516</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>23</v>
+        <v>197</v>
+      </c>
+      <c r="C97" s="11">
+        <v>21.886589050292969</v>
+      </c>
+      <c r="D97" s="12">
+        <v>21.889556884765625</v>
+      </c>
+      <c r="E97" s="12">
+        <v>21.885984420776367</v>
+      </c>
+      <c r="F97" s="12">
+        <v>21.890302658081055</v>
+      </c>
+      <c r="G97" s="12">
+        <v>21.891286849975586</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C98" s="11">
-        <v>21.886589050292969</v>
+        <v>21.885196685791016</v>
       </c>
       <c r="D98" s="12">
-        <v>21.889556884765625</v>
+        <v>21.889060974121094</v>
       </c>
       <c r="E98" s="12">
-        <v>21.885984420776367</v>
+        <v>21.884433746337891</v>
       </c>
       <c r="F98" s="12">
-        <v>21.890302658081055</v>
+        <v>21.888387680053711</v>
       </c>
       <c r="G98" s="12">
-        <v>21.891286849975586</v>
+        <v>21.889049530029297</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C99" s="11">
-        <v>21.885196685791016</v>
+        <v>21.888345718383789</v>
       </c>
       <c r="D99" s="12">
-        <v>21.889060974121094</v>
+        <v>21.890129089355469</v>
       </c>
       <c r="E99" s="12">
-        <v>21.884433746337891</v>
+        <v>21.8878173828125</v>
       </c>
       <c r="F99" s="12">
-        <v>21.888387680053711</v>
+        <v>21.893096923828125</v>
       </c>
       <c r="G99" s="12">
-        <v>21.889049530029297</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C100" s="11">
-        <v>21.888345718383789</v>
-      </c>
-      <c r="D100" s="12">
-        <v>21.890129089355469</v>
-      </c>
-      <c r="E100" s="12">
-        <v>21.8878173828125</v>
-      </c>
-      <c r="F100" s="12">
-        <v>21.893096923828125</v>
-      </c>
-      <c r="G100" s="12">
         <v>21.892501831054688</v>
       </c>
     </row>
+    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4250,11 +4192,9 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -4280,15 +4220,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>30.914709091186523</v>
@@ -4296,7 +4236,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>29.892593383789062</v>
@@ -4304,7 +4244,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4">
         <v>29.894725799560547</v>
@@ -4312,7 +4252,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4">
         <v>32.885646820068359</v>
@@ -4320,7 +4260,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>31.923347473144531</v>
@@ -4328,7 +4268,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4">
         <v>30.947450637817383</v>
@@ -4336,7 +4276,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4">
         <v>30.898262023925781</v>
@@ -4344,7 +4284,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4">
         <v>31.886405944824219</v>
@@ -4352,7 +4292,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4">
         <v>30.895318984985352</v>
@@ -4360,7 +4300,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4">
         <v>31.918970108032227</v>
@@ -4368,7 +4308,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4">
         <v>30.8929443359375</v>
@@ -4376,7 +4316,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="4">
         <v>29.893756866455078</v>
@@ -4384,7 +4324,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4">
         <v>28.907720565795898</v>
@@ -4392,7 +4332,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4">
         <v>32.915229797363281</v>
@@ -4400,7 +4340,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" s="4">
         <v>31.933006286621094</v>
@@ -4408,7 +4348,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4">
         <v>30.955327987670898</v>
@@ -4416,7 +4356,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4">
         <v>29.900350570678711</v>
@@ -4424,7 +4364,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4">
         <v>30.906478881835938</v>
@@ -4432,7 +4372,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4">
         <v>30.015558242797852</v>
@@ -4440,7 +4380,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4">
         <v>29.908964157104492</v>
@@ -4448,7 +4388,7 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4">
         <v>30.877904891967773</v>
@@ -4456,7 +4396,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4">
         <v>31.898872375488281</v>
@@ -4464,7 +4404,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B25" s="4">
         <v>32.899791717529297</v>
@@ -4472,7 +4412,7 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B26" s="4">
         <v>31.900041580200195</v>
@@ -4480,7 +4420,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="4">
         <v>30.899215698242188</v>
@@ -4488,7 +4428,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="4">
         <v>31.878820419311523</v>
@@ -4496,7 +4436,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B29" s="4">
         <v>28.89484977722168</v>
@@ -4504,7 +4444,7 @@
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B30" s="4">
         <v>31.881462097167969</v>
@@ -4512,7 +4452,7 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B31" s="4">
         <v>29.897172927856445</v>
@@ -4520,7 +4460,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B32" s="4">
         <v>29.894147872924805</v>
@@ -4528,7 +4468,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" s="4">
         <v>31.873043060302734</v>
@@ -4536,7 +4476,7 @@
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" s="4">
         <v>30.891448974609375</v>
@@ -4544,7 +4484,7 @@
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B35" s="4">
         <v>30.897619247436523</v>
@@ -4552,7 +4492,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" s="4">
         <v>30.900562286376953</v>
@@ -4560,7 +4500,7 @@
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" s="4">
         <v>29.881351470947266</v>
@@ -4568,7 +4508,7 @@
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" s="4">
         <v>32.893413543701172</v>
@@ -4576,7 +4516,7 @@
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B39" s="4">
         <v>30.899877548217773</v>
@@ -4584,7 +4524,7 @@
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B40" s="4">
         <v>29.900217056274414</v>
@@ -4592,7 +4532,7 @@
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B41" s="4">
         <v>30.901157379150391</v>
@@ -4600,7 +4540,7 @@
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B42" s="4">
         <v>29.90745735168457</v>
@@ -4608,7 +4548,7 @@
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4">
         <v>30.895229339599609</v>
@@ -4616,7 +4556,7 @@
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B44" s="4">
         <v>29.884521484375</v>
@@ -4624,7 +4564,7 @@
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4">
         <v>31.918445587158203</v>
@@ -4632,7 +4572,7 @@
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B46" s="4">
         <v>30.92442512512207</v>
@@ -4640,7 +4580,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B47" s="4">
         <v>32.91314697265625</v>
@@ -4648,7 +4588,7 @@
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B48" s="4">
         <v>30.918905258178711</v>
@@ -4656,7 +4596,7 @@
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B49" s="4">
         <v>29.917095184326172</v>
@@ -4664,7 +4604,7 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B50" s="4">
         <v>31.908161163330078</v>
@@ -4672,7 +4612,7 @@
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B51" s="4">
         <v>29.913234710693359</v>
@@ -4680,7 +4620,7 @@
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B52" s="4">
         <v>30.884122848510742</v>
@@ -4688,7 +4628,7 @@
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B53" s="4">
         <v>30.917659759521484</v>
@@ -4696,7 +4636,7 @@
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B54" s="4">
         <v>29.908811569213867</v>
@@ -4704,7 +4644,7 @@
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B55" s="4">
         <v>29.892829895019531</v>
@@ -4712,7 +4652,7 @@
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B56" s="4">
         <v>29.896526336669922</v>
@@ -4720,7 +4660,7 @@
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B57" s="4">
         <v>30.896093368530273</v>
@@ -4728,7 +4668,7 @@
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B58" s="4">
         <v>29.888259887695312</v>
@@ -4736,7 +4676,7 @@
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B59" s="4">
         <v>29.89727783203125</v>
@@ -4744,7 +4684,7 @@
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B60" s="4">
         <v>33.921558380126953</v>
@@ -4752,7 +4692,7 @@
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B61" s="4">
         <v>29.895294189453125</v>
@@ -4760,7 +4700,7 @@
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B62" s="4">
         <v>30.923200607299805</v>
@@ -4768,7 +4708,7 @@
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B63" s="4">
         <v>31.893083572387695</v>
@@ -4776,7 +4716,7 @@
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B64" s="4">
         <v>30.898645401000977</v>
@@ -4784,7 +4724,7 @@
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B65" s="4">
         <v>29.902156829833984</v>
@@ -4792,7 +4732,7 @@
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B66" s="4">
         <v>30.891826629638672</v>
@@ -4800,7 +4740,7 @@
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B67" s="4">
         <v>29.897747039794922</v>
@@ -4808,7 +4748,7 @@
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B68" s="4">
         <v>30.894525527954102</v>
@@ -4816,7 +4756,7 @@
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B69" s="4">
         <v>29.8870849609375</v>
@@ -4824,7 +4764,7 @@
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B70" s="4">
         <v>29.895362854003906</v>
@@ -4832,7 +4772,7 @@
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B71" s="4">
         <v>30.885660171508789</v>
@@ -4840,7 +4780,7 @@
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B72" s="4">
         <v>29.884965896606445</v>
@@ -4848,7 +4788,7 @@
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B73" s="4">
         <v>30.880331039428711</v>
@@ -4856,7 +4796,7 @@
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B74" s="4">
         <v>31.892080307006836</v>
@@ -4864,7 +4804,7 @@
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B75" s="4">
         <v>28.896696090698242</v>
@@ -4872,7 +4812,7 @@
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B76" s="4">
         <v>30.887510299682617</v>
@@ -4880,7 +4820,7 @@
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B77" s="4">
         <v>30.925548553466797</v>
@@ -4888,15 +4828,15 @@
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B79" s="4">
         <v>29.899961471557617</v>
@@ -4904,7 +4844,7 @@
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B80" s="4">
         <v>29.893932342529297</v>
@@ -4912,7 +4852,7 @@
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B81" s="4">
         <v>29.902708053588867</v>
@@ -4920,7 +4860,7 @@
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B82" s="4">
         <v>33.893535614013672</v>
@@ -4928,7 +4868,7 @@
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B83" s="4">
         <v>30.882589340209961</v>
@@ -4936,7 +4876,7 @@
     </row>
     <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B84" s="4">
         <v>30.881217956542969</v>
@@ -4944,7 +4884,7 @@
     </row>
     <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B85" s="4">
         <v>30.893064498901367</v>
@@ -4952,7 +4892,7 @@
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B86" s="4">
         <v>28.890214920043945</v>
@@ -4960,7 +4900,7 @@
     </row>
     <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B87" s="4">
         <v>27.890878677368164</v>
@@ -4968,7 +4908,7 @@
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B88" s="4">
         <v>27.904565811157227</v>
@@ -4976,7 +4916,7 @@
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B89" s="4">
         <v>26.905902862548828</v>
@@ -4984,7 +4924,7 @@
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B90" s="4">
         <v>31.900989532470703</v>
@@ -4992,7 +4932,7 @@
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B91" s="4">
         <v>28.902608871459961</v>
@@ -5000,7 +4940,7 @@
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B92" s="4">
         <v>29.915422439575195</v>
@@ -5008,31 +4948,31 @@
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B96" s="4">
         <v>21.886589050292969</v>
@@ -5040,7 +4980,7 @@
     </row>
     <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B97" s="4">
         <v>21.885196685791016</v>
@@ -5048,7 +4988,7 @@
     </row>
     <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B98" s="4">
         <v>21.888345718383789</v>

</xml_diff>